<commit_message>
test: Fix testdata in qubit flex 2 parser (#607)
Example 2 input data had mis-aligned columns, leading to some incorrect
results.
</commit_message>
<xml_diff>
--- a/tests/parsers/thermo_fisher_qubit_flex/testdata/thermo_fisher_qubit_flex_example_02.xlsx
+++ b/tests/parsers/thermo_fisher_qubit_flex/testdata/thermo_fisher_qubit_flex_example_02.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="80">
   <si>
     <t>Run ID</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>Std 1 RFU</t>
+  </si>
+  <si>
+    <t>Std 2 RFU</t>
   </si>
   <si>
     <t>Std 3 RFU</t>
@@ -289,9 +292,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
@@ -570,2731 +579,2736 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="A2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="4">
         <v>44996.42888888889</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="1">
+      <c r="D2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="3">
         <v>8.09</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="1">
+      <c r="F2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="3">
         <v>80.9</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="1">
+      <c r="H2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="3">
         <v>2.0</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="3">
         <v>100.0</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="K2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="L2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="M2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O2" s="1">
+      <c r="N2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="3">
         <v>1.76123674997</v>
       </c>
-      <c r="P2" s="1">
+      <c r="P2" s="3">
         <v>968.243447194</v>
       </c>
-      <c r="R2" s="1">
+      <c r="R2" s="3">
         <v>156.0</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="A3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="4">
         <v>44996.42888888889</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="C3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="3">
+        <v>8.15</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="3">
+        <v>81.5</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="J3" s="3">
+        <v>100.0</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="1">
-        <v>8.15</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="1">
-        <v>81.5</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="J3" s="1">
-        <v>100.0</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O3" s="1">
+      <c r="O3" s="3">
         <v>1.83263823983</v>
       </c>
-      <c r="P3" s="1">
+      <c r="P3" s="3">
         <v>1011.24211785</v>
       </c>
-      <c r="R3" s="1">
+      <c r="R3" s="3">
         <v>164.0</v>
       </c>
-      <c r="S3" s="2">
+      <c r="S3" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="A4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="4">
         <v>44996.42888888889</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="1">
+      <c r="C4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="3">
         <v>8.1</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="1">
+      <c r="F4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="3">
         <v>81.0</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="1">
+      <c r="H4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="3">
         <v>2.0</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="3">
         <v>100.0</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" s="1" t="s">
+      <c r="K4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="L4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="M4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O4" s="1">
+      <c r="N4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" s="3">
         <v>1.78503724659</v>
       </c>
-      <c r="P4" s="1">
+      <c r="P4" s="3">
         <v>967.148849047</v>
       </c>
-      <c r="R4" s="1">
+      <c r="R4" s="3">
         <v>156.0</v>
       </c>
-      <c r="S4" s="2">
+      <c r="S4" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="A5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="4">
         <v>44996.42888888889</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="1">
+      <c r="C5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="3">
         <v>8.27</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="1">
+      <c r="F5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="3">
         <v>82.7</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="1">
+      <c r="H5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="3">
         <v>2.0</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="3">
         <v>100.0</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L5" s="1" t="s">
+      <c r="K5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="L5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="M5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O5" s="1">
+      <c r="N5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5" s="3">
         <v>1.80883774321</v>
       </c>
-      <c r="P5" s="1">
+      <c r="P5" s="3">
         <v>982.615996767</v>
       </c>
-      <c r="R5" s="1">
+      <c r="R5" s="3">
         <v>162.0</v>
       </c>
-      <c r="S5" s="2">
+      <c r="S5" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="2">
+      <c r="A6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="4">
         <v>44996.42888888889</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="1">
+      <c r="C6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="3">
         <v>7.85</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="1">
+      <c r="F6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="3">
         <v>78.5</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="1">
+      <c r="H6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="3">
         <v>2.0</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="3">
         <v>100.0</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L6" s="1" t="s">
+      <c r="K6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="L6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="M6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O6" s="1">
+      <c r="N6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O6" s="3">
         <v>1.76123674997</v>
       </c>
-      <c r="P6" s="1">
+      <c r="P6" s="3">
         <v>957.939947254</v>
       </c>
-      <c r="R6" s="1">
+      <c r="R6" s="3">
         <v>150.0</v>
       </c>
-      <c r="S6" s="2">
+      <c r="S6" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="2">
+      <c r="A7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="4">
         <v>44996.42888888889</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="1">
+      <c r="C7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="3">
         <v>7.75</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="1">
+      <c r="F7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="3">
         <v>77.5</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="1">
+      <c r="H7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="3">
         <v>2.0</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="3">
         <v>100.0</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L7" s="1" t="s">
+      <c r="K7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="L7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="M7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O7" s="1">
+      <c r="N7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O7" s="3">
         <v>1.66603476348</v>
       </c>
-      <c r="P7" s="1">
+      <c r="P7" s="3">
         <v>855.35706446</v>
       </c>
-      <c r="R7" s="1">
+      <c r="R7" s="3">
         <v>132.0</v>
       </c>
-      <c r="S7" s="2">
+      <c r="S7" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="2">
+      <c r="A8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="4">
         <v>44996.42888888889</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="1">
+      <c r="C8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="3">
         <v>7.71</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="1">
+      <c r="F8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="3">
         <v>77.1</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I8" s="1">
+      <c r="H8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="3">
         <v>2.0</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="3">
         <v>100.0</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L8" s="1" t="s">
+      <c r="K8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="L8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="M8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O8" s="1">
+      <c r="N8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O8" s="3">
         <v>1.47563079051</v>
       </c>
-      <c r="P8" s="1">
+      <c r="P8" s="3">
         <v>814.547590094</v>
       </c>
-      <c r="R8" s="1">
+      <c r="R8" s="3">
         <v>125.0</v>
       </c>
-      <c r="S8" s="2">
+      <c r="S8" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="2">
+      <c r="A9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="4">
         <v>44996.42888888889</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="1">
+      <c r="C9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="3">
         <v>7.17</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="1">
+      <c r="F9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="3">
         <v>71.7</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" s="1">
+      <c r="H9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="3">
         <v>2.0</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="3">
         <v>100.0</v>
       </c>
-      <c r="K9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L9" s="1" t="s">
+      <c r="K9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="L9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="M9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O9" s="1">
+      <c r="N9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O9" s="3">
         <v>1.49943128713</v>
       </c>
-      <c r="P9" s="1">
+      <c r="P9" s="3">
         <v>790.63300016</v>
       </c>
-      <c r="R9" s="1">
+      <c r="R9" s="3">
         <v>113.0</v>
       </c>
-      <c r="S9" s="2">
+      <c r="S9" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="2">
+      <c r="A10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="4">
         <v>44996.42903935185</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="1">
+      <c r="C10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="3">
         <v>6.93</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="1">
+      <c r="F10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="3">
         <v>69.3</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I10" s="1">
+      <c r="H10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="3">
         <v>2.0</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="3">
         <v>100.0</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L10" s="1" t="s">
+      <c r="K10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="L10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="M10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O10" s="1">
+      <c r="N10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O10" s="3">
         <v>1.76123674997</v>
       </c>
-      <c r="P10" s="1">
+      <c r="P10" s="3">
         <v>968.243447194</v>
       </c>
-      <c r="R10" s="1">
+      <c r="R10" s="3">
         <v>134.0</v>
       </c>
-      <c r="S10" s="2">
+      <c r="S10" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="2">
+      <c r="A11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="4">
         <v>44996.42903935185</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="1">
+      <c r="C11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="3">
         <v>6.91</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="1">
+      <c r="F11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="3">
         <v>69.1</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I11" s="1">
+      <c r="H11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" s="3">
         <v>2.0</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="3">
         <v>100.0</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L11" s="1" t="s">
+      <c r="K11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="L11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N11" s="1" t="s">
+      <c r="M11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O11" s="1">
+      <c r="N11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O11" s="3">
         <v>1.83263823983</v>
       </c>
-      <c r="P11" s="1">
+      <c r="P11" s="3">
         <v>1011.24211785</v>
       </c>
-      <c r="R11" s="1">
+      <c r="R11" s="3">
         <v>139.0</v>
       </c>
-      <c r="S11" s="2">
+      <c r="S11" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="2">
+      <c r="A12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="4">
         <v>44996.42903935185</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="1">
+      <c r="C12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="3">
         <v>7.02</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="1">
+      <c r="F12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="3">
         <v>70.2</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I12" s="1">
+      <c r="H12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="3">
         <v>2.0</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="3">
         <v>100.0</v>
       </c>
-      <c r="K12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L12" s="1" t="s">
+      <c r="K12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="L12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N12" s="1" t="s">
+      <c r="M12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O12" s="1">
+      <c r="N12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O12" s="3">
         <v>1.78503724659</v>
       </c>
-      <c r="P12" s="1">
+      <c r="P12" s="3">
         <v>967.148849047</v>
       </c>
-      <c r="R12" s="1">
+      <c r="R12" s="3">
         <v>135.0</v>
       </c>
-      <c r="S12" s="2">
+      <c r="S12" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="2">
+      <c r="A13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="4">
         <v>44996.42903935185</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="1">
+      <c r="C13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="3">
         <v>7.04</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="1">
+      <c r="F13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="3">
         <v>70.4</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I13" s="1">
+      <c r="H13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="3">
         <v>2.0</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13" s="3">
         <v>100.0</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L13" s="1" t="s">
+      <c r="K13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="L13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N13" s="1" t="s">
+      <c r="M13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O13" s="1">
+      <c r="N13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O13" s="3">
         <v>1.80883774321</v>
       </c>
-      <c r="P13" s="1">
+      <c r="P13" s="3">
         <v>982.615996767</v>
       </c>
-      <c r="R13" s="1">
+      <c r="R13" s="3">
         <v>138.0</v>
       </c>
-      <c r="S13" s="2">
+      <c r="S13" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="2">
+      <c r="A14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="4">
         <v>44996.42903935185</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="1">
+      <c r="C14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="3">
         <v>7.01</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="1">
+      <c r="F14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="3">
         <v>70.1</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I14" s="1">
+      <c r="H14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="3">
         <v>2.0</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14" s="3">
         <v>100.0</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L14" s="1" t="s">
+      <c r="K14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="L14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N14" s="1" t="s">
+      <c r="M14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O14" s="1">
+      <c r="N14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O14" s="3">
         <v>1.76123674997</v>
       </c>
-      <c r="P14" s="1">
+      <c r="P14" s="3">
         <v>957.939947254</v>
       </c>
-      <c r="R14" s="1">
+      <c r="R14" s="3">
         <v>134.0</v>
       </c>
-      <c r="S14" s="2">
+      <c r="S14" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="2">
+      <c r="A15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="4">
         <v>44996.42903935185</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="1">
+      <c r="C15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="3">
         <v>7.28</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G15" s="1">
+      <c r="F15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="3">
         <v>72.8</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I15" s="1">
+      <c r="H15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="3">
         <v>2.0</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15" s="3">
         <v>100.0</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L15" s="1" t="s">
+      <c r="K15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M15" s="1" t="s">
+      <c r="L15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N15" s="1" t="s">
+      <c r="M15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O15" s="1">
+      <c r="N15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O15" s="3">
         <v>1.66603476348</v>
       </c>
-      <c r="P15" s="1">
+      <c r="P15" s="3">
         <v>855.35706446</v>
       </c>
-      <c r="R15" s="1">
+      <c r="R15" s="3">
         <v>124.0</v>
       </c>
-      <c r="S15" s="2">
+      <c r="S15" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="2">
+      <c r="A16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="4">
         <v>44996.42903935185</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="1">
+      <c r="C16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="3">
         <v>7.16</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="1">
+      <c r="F16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="3">
         <v>71.6</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I16" s="1">
+      <c r="H16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" s="3">
         <v>2.0</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J16" s="3">
         <v>100.0</v>
       </c>
-      <c r="K16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L16" s="1" t="s">
+      <c r="K16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M16" s="1" t="s">
+      <c r="L16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N16" s="1" t="s">
+      <c r="M16" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O16" s="1">
+      <c r="N16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O16" s="3">
         <v>1.47563079051</v>
       </c>
-      <c r="P16" s="1">
+      <c r="P16" s="3">
         <v>814.547590094</v>
       </c>
-      <c r="R16" s="1">
+      <c r="R16" s="3">
         <v>116.0</v>
       </c>
-      <c r="S16" s="2">
+      <c r="S16" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="2">
+      <c r="A17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="4">
         <v>44996.42903935185</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" s="1">
+      <c r="C17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="3">
         <v>7.03</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G17" s="1">
+      <c r="F17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="3">
         <v>70.3</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I17" s="1">
+      <c r="H17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" s="3">
         <v>2.0</v>
       </c>
-      <c r="J17" s="1">
+      <c r="J17" s="3">
         <v>100.0</v>
       </c>
-      <c r="K17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L17" s="1" t="s">
+      <c r="K17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="L17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N17" s="1" t="s">
+      <c r="M17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O17" s="1">
+      <c r="N17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O17" s="3">
         <v>1.49943128713</v>
       </c>
-      <c r="P17" s="1">
+      <c r="P17" s="3">
         <v>790.63300016</v>
       </c>
-      <c r="R17" s="1">
+      <c r="R17" s="3">
         <v>111.0</v>
       </c>
-      <c r="S17" s="2">
+      <c r="S17" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="2">
+      <c r="A18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="4">
         <v>44996.429143518515</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="1">
+      <c r="C18" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="3">
         <v>7.47</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G18" s="1">
+      <c r="F18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="3">
         <v>74.7</v>
       </c>
-      <c r="H18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I18" s="1">
+      <c r="H18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" s="3">
         <v>2.0</v>
       </c>
-      <c r="J18" s="1">
+      <c r="J18" s="3">
         <v>100.0</v>
       </c>
-      <c r="K18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L18" s="1" t="s">
+      <c r="K18" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M18" s="1" t="s">
+      <c r="L18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N18" s="1" t="s">
+      <c r="M18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O18" s="1">
+      <c r="N18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O18" s="3">
         <v>1.76123674997</v>
       </c>
-      <c r="P18" s="1">
+      <c r="P18" s="3">
         <v>968.243447194</v>
       </c>
-      <c r="R18" s="1">
+      <c r="R18" s="3">
         <v>144.0</v>
       </c>
-      <c r="S18" s="2">
+      <c r="S18" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="2">
+      <c r="A19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="4">
         <v>44996.429143518515</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="1">
+      <c r="C19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="3">
         <v>7.19</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G19" s="1">
+      <c r="F19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" s="3">
         <v>71.9</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I19" s="1">
+      <c r="H19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19" s="3">
         <v>2.0</v>
       </c>
-      <c r="J19" s="1">
+      <c r="J19" s="3">
         <v>100.0</v>
       </c>
-      <c r="K19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L19" s="1" t="s">
+      <c r="K19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="L19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N19" s="1" t="s">
+      <c r="M19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O19" s="1">
+      <c r="N19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O19" s="3">
         <v>1.83263823983</v>
       </c>
-      <c r="P19" s="1">
+      <c r="P19" s="3">
         <v>1011.24211785</v>
       </c>
-      <c r="R19" s="1">
+      <c r="R19" s="3">
         <v>145.0</v>
       </c>
-      <c r="S19" s="2">
+      <c r="S19" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="2">
+      <c r="A20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="4">
         <v>44996.429143518515</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="1">
+      <c r="C20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="3">
         <v>7.35</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G20" s="1">
+      <c r="F20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="3">
         <v>73.5</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I20" s="1">
+      <c r="H20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="3">
         <v>2.0</v>
       </c>
-      <c r="J20" s="1">
+      <c r="J20" s="3">
         <v>100.0</v>
       </c>
-      <c r="K20" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L20" s="1" t="s">
+      <c r="K20" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="L20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N20" s="1" t="s">
+      <c r="M20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O20" s="1">
+      <c r="N20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O20" s="3">
         <v>1.78503724659</v>
       </c>
-      <c r="P20" s="1">
+      <c r="P20" s="3">
         <v>967.148849047</v>
       </c>
-      <c r="R20" s="1">
+      <c r="R20" s="3">
         <v>142.0</v>
       </c>
-      <c r="S20" s="2">
+      <c r="S20" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="2">
+      <c r="A21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="4">
         <v>44996.429143518515</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E21" s="1">
+      <c r="C21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="3">
         <v>7.36</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G21" s="1">
+      <c r="F21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" s="3">
         <v>73.6</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I21" s="1">
+      <c r="H21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" s="3">
         <v>2.0</v>
       </c>
-      <c r="J21" s="1">
+      <c r="J21" s="3">
         <v>100.0</v>
       </c>
-      <c r="K21" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L21" s="1" t="s">
+      <c r="K21" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M21" s="1" t="s">
+      <c r="L21" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N21" s="1" t="s">
+      <c r="M21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O21" s="1">
+      <c r="N21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O21" s="3">
         <v>1.80883774321</v>
       </c>
-      <c r="P21" s="1">
+      <c r="P21" s="3">
         <v>982.615996767</v>
       </c>
-      <c r="R21" s="1">
+      <c r="R21" s="3">
         <v>144.0</v>
       </c>
-      <c r="S21" s="2">
+      <c r="S21" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="2">
+      <c r="A22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="4">
         <v>44996.429143518515</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E22" s="1">
+      <c r="C22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="3">
         <v>6.95</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G22" s="1">
+      <c r="F22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" s="3">
         <v>69.5</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I22" s="1">
+      <c r="H22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="3">
         <v>2.0</v>
       </c>
-      <c r="J22" s="1">
+      <c r="J22" s="3">
         <v>100.0</v>
       </c>
-      <c r="K22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L22" s="1" t="s">
+      <c r="K22" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M22" s="1" t="s">
+      <c r="L22" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N22" s="1" t="s">
+      <c r="M22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O22" s="1">
+      <c r="N22" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O22" s="3">
         <v>1.76123674997</v>
       </c>
-      <c r="P22" s="1">
+      <c r="P22" s="3">
         <v>957.939947254</v>
       </c>
-      <c r="R22" s="1">
+      <c r="R22" s="3">
         <v>133.0</v>
       </c>
-      <c r="S22" s="2">
+      <c r="S22" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="2">
+      <c r="A23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="4">
         <v>44996.429143518515</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E23" s="1">
+      <c r="C23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E23" s="3">
         <v>7.06</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G23" s="1">
+      <c r="F23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" s="3">
         <v>70.6</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I23" s="1">
+      <c r="H23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23" s="3">
         <v>2.0</v>
       </c>
-      <c r="J23" s="1">
+      <c r="J23" s="3">
         <v>100.0</v>
       </c>
-      <c r="K23" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L23" s="1" t="s">
+      <c r="K23" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="L23" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N23" s="1" t="s">
+      <c r="M23" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O23" s="1">
+      <c r="N23" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O23" s="3">
         <v>1.66603476348</v>
       </c>
-      <c r="P23" s="1">
+      <c r="P23" s="3">
         <v>855.35706446</v>
       </c>
-      <c r="R23" s="1">
+      <c r="R23" s="3">
         <v>120.0</v>
       </c>
-      <c r="S23" s="2">
+      <c r="S23" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="2">
+      <c r="A24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="4">
         <v>44996.429143518515</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E24" s="1">
+      <c r="C24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="3">
         <v>6.94</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G24" s="1">
+      <c r="F24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G24" s="3">
         <v>69.4</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I24" s="1">
+      <c r="H24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" s="3">
         <v>2.0</v>
       </c>
-      <c r="J24" s="1">
+      <c r="J24" s="3">
         <v>100.0</v>
       </c>
-      <c r="K24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L24" s="1" t="s">
+      <c r="K24" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M24" s="1" t="s">
+      <c r="L24" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N24" s="1" t="s">
+      <c r="M24" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O24" s="1">
+      <c r="N24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O24" s="3">
         <v>1.47563079051</v>
       </c>
-      <c r="P24" s="1">
+      <c r="P24" s="3">
         <v>814.547590094</v>
       </c>
-      <c r="R24" s="1">
+      <c r="R24" s="3">
         <v>113.0</v>
       </c>
-      <c r="S24" s="2">
+      <c r="S24" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="2">
+      <c r="A25" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="4">
         <v>44996.429143518515</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E25" s="1">
+      <c r="C25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="3">
         <v>7.01</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G25" s="1">
+      <c r="F25" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G25" s="3">
         <v>70.1</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I25" s="1">
+      <c r="H25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I25" s="3">
         <v>2.0</v>
       </c>
-      <c r="J25" s="1">
+      <c r="J25" s="3">
         <v>100.0</v>
       </c>
-      <c r="K25" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L25" s="1" t="s">
+      <c r="K25" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M25" s="1" t="s">
+      <c r="L25" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N25" s="1" t="s">
+      <c r="M25" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O25" s="1">
+      <c r="N25" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O25" s="3">
         <v>1.49943128713</v>
       </c>
-      <c r="P25" s="1">
+      <c r="P25" s="3">
         <v>790.63300016</v>
       </c>
-      <c r="R25" s="1">
+      <c r="R25" s="3">
         <v>110.0</v>
       </c>
-      <c r="S25" s="2">
+      <c r="S25" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" s="2">
+      <c r="A26" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="4">
         <v>44996.429236111115</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E26" s="1">
+      <c r="C26" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="3">
         <v>6.63</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G26" s="1">
+      <c r="F26" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G26" s="3">
         <v>66.3</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I26" s="1">
+      <c r="H26" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26" s="3">
         <v>2.0</v>
       </c>
-      <c r="J26" s="1">
+      <c r="J26" s="3">
         <v>100.0</v>
       </c>
-      <c r="K26" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L26" s="1" t="s">
+      <c r="K26" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M26" s="1" t="s">
+      <c r="L26" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N26" s="1" t="s">
+      <c r="M26" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O26" s="1">
+      <c r="N26" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O26" s="3">
         <v>1.76123674997</v>
       </c>
-      <c r="P26" s="1">
+      <c r="P26" s="3">
         <v>968.243447194</v>
       </c>
-      <c r="R26" s="1">
+      <c r="R26" s="3">
         <v>128.0</v>
       </c>
-      <c r="S26" s="2">
+      <c r="S26" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="2">
+      <c r="A27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="4">
         <v>44996.429236111115</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E27" s="1">
+      <c r="C27" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E27" s="3">
         <v>6.47</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G27" s="1">
+      <c r="F27" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" s="3">
         <v>64.7</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I27" s="1">
+      <c r="H27" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I27" s="3">
         <v>2.0</v>
       </c>
-      <c r="J27" s="1">
+      <c r="J27" s="3">
         <v>100.0</v>
       </c>
-      <c r="K27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L27" s="1" t="s">
+      <c r="K27" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M27" s="1" t="s">
+      <c r="L27" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N27" s="1" t="s">
+      <c r="M27" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O27" s="1">
+      <c r="N27" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O27" s="3">
         <v>1.83263823983</v>
       </c>
-      <c r="P27" s="1">
+      <c r="P27" s="3">
         <v>1011.24211785</v>
       </c>
-      <c r="R27" s="1">
+      <c r="R27" s="3">
         <v>130.0</v>
       </c>
-      <c r="S27" s="2">
+      <c r="S27" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" s="2">
+      <c r="A28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="4">
         <v>44996.429236111115</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E28" s="1">
+      <c r="C28" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" s="3">
         <v>6.48</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G28" s="1">
+      <c r="F28" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" s="3">
         <v>64.8</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I28" s="1">
+      <c r="H28" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I28" s="3">
         <v>2.0</v>
       </c>
-      <c r="J28" s="1">
+      <c r="J28" s="3">
         <v>100.0</v>
       </c>
-      <c r="K28" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L28" s="1" t="s">
+      <c r="K28" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M28" s="1" t="s">
+      <c r="L28" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N28" s="1" t="s">
+      <c r="M28" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O28" s="1">
+      <c r="N28" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O28" s="3">
         <v>1.78503724659</v>
       </c>
-      <c r="P28" s="1">
+      <c r="P28" s="3">
         <v>967.148849047</v>
       </c>
-      <c r="R28" s="1">
+      <c r="R28" s="3">
         <v>125.0</v>
       </c>
-      <c r="S28" s="2">
+      <c r="S28" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="2">
+      <c r="A29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="4">
         <v>44996.429236111115</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E29" s="1">
+      <c r="C29" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" s="3">
         <v>6.49</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G29" s="1">
+      <c r="F29" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G29" s="3">
         <v>64.9</v>
       </c>
-      <c r="H29" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I29" s="1">
+      <c r="H29" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I29" s="3">
         <v>2.0</v>
       </c>
-      <c r="J29" s="1">
+      <c r="J29" s="3">
         <v>100.0</v>
       </c>
-      <c r="K29" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L29" s="1" t="s">
+      <c r="K29" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M29" s="1" t="s">
+      <c r="L29" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N29" s="1" t="s">
+      <c r="M29" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O29" s="1">
+      <c r="N29" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O29" s="3">
         <v>1.80883774321</v>
       </c>
-      <c r="P29" s="1">
+      <c r="P29" s="3">
         <v>982.615996767</v>
       </c>
-      <c r="R29" s="1">
+      <c r="R29" s="3">
         <v>127.0</v>
       </c>
-      <c r="S29" s="2">
+      <c r="S29" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B30" s="2">
+      <c r="A30" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="4">
         <v>44996.429236111115</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E30" s="1">
+      <c r="C30" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="3">
         <v>6.45</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G30" s="1">
+      <c r="F30" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G30" s="3">
         <v>64.5</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I30" s="1">
+      <c r="H30" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I30" s="3">
         <v>2.0</v>
       </c>
-      <c r="J30" s="1">
+      <c r="J30" s="3">
         <v>100.0</v>
       </c>
-      <c r="K30" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L30" s="1" t="s">
+      <c r="K30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M30" s="1" t="s">
+      <c r="L30" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N30" s="1" t="s">
+      <c r="M30" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O30" s="1">
+      <c r="N30" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O30" s="3">
         <v>1.76123674997</v>
       </c>
-      <c r="P30" s="1">
+      <c r="P30" s="3">
         <v>957.939947254</v>
       </c>
-      <c r="R30" s="1">
+      <c r="R30" s="3">
         <v>123.0</v>
       </c>
-      <c r="S30" s="2">
+      <c r="S30" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" s="2">
+      <c r="A31" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="4">
         <v>44996.429236111115</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E31" s="1">
+      <c r="C31" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31" s="3">
         <v>6.53</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G31" s="1">
+      <c r="F31" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G31" s="3">
         <v>65.3</v>
       </c>
-      <c r="H31" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I31" s="1">
+      <c r="H31" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I31" s="3">
         <v>2.0</v>
       </c>
-      <c r="J31" s="1">
+      <c r="J31" s="3">
         <v>100.0</v>
       </c>
-      <c r="K31" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L31" s="1" t="s">
+      <c r="K31" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M31" s="1" t="s">
+      <c r="L31" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N31" s="1" t="s">
+      <c r="M31" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O31" s="1">
+      <c r="N31" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O31" s="3">
         <v>1.66603476348</v>
       </c>
-      <c r="P31" s="1">
+      <c r="P31" s="3">
         <v>855.35706446</v>
       </c>
-      <c r="R31" s="1">
+      <c r="R31" s="3">
         <v>111.0</v>
       </c>
-      <c r="S31" s="2">
+      <c r="S31" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B32" s="2">
+      <c r="A32" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="4">
         <v>44996.429236111115</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E32" s="1">
+      <c r="C32" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E32" s="3">
         <v>6.56</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G32" s="1">
+      <c r="F32" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G32" s="3">
         <v>65.6</v>
       </c>
-      <c r="H32" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I32" s="1">
+      <c r="H32" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I32" s="3">
         <v>2.0</v>
       </c>
-      <c r="J32" s="1">
+      <c r="J32" s="3">
         <v>100.0</v>
       </c>
-      <c r="K32" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L32" s="1" t="s">
+      <c r="K32" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M32" s="1" t="s">
+      <c r="L32" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N32" s="1" t="s">
+      <c r="M32" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O32" s="1">
+      <c r="N32" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O32" s="3">
         <v>1.47563079051</v>
       </c>
-      <c r="P32" s="1">
+      <c r="P32" s="3">
         <v>814.547590094</v>
       </c>
-      <c r="R32" s="1">
+      <c r="R32" s="3">
         <v>106.0</v>
       </c>
-      <c r="S32" s="2">
+      <c r="S32" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B33" s="2">
+      <c r="A33" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="4">
         <v>44996.429236111115</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E33" s="1">
+      <c r="C33" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E33" s="3">
         <v>6.59</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G33" s="1">
+      <c r="F33" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G33" s="3">
         <v>65.9</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I33" s="1">
+      <c r="H33" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I33" s="3">
         <v>2.0</v>
       </c>
-      <c r="J33" s="1">
+      <c r="J33" s="3">
         <v>100.0</v>
       </c>
-      <c r="K33" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L33" s="1" t="s">
+      <c r="K33" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M33" s="1" t="s">
+      <c r="L33" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N33" s="1" t="s">
+      <c r="M33" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O33" s="1">
+      <c r="N33" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O33" s="3">
         <v>1.49943128713</v>
       </c>
-      <c r="P33" s="1">
+      <c r="P33" s="3">
         <v>790.63300016</v>
       </c>
-      <c r="R33" s="1">
+      <c r="R33" s="3">
         <v>104.0</v>
       </c>
-      <c r="S33" s="2">
+      <c r="S33" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="2">
+      <c r="A34" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="4">
         <v>44996.42934027778</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E34" s="1">
+      <c r="C34" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E34" s="3">
         <v>6.54</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G34" s="1">
+      <c r="F34" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G34" s="3">
         <v>65.4</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I34" s="1">
+      <c r="H34" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I34" s="3">
         <v>2.0</v>
       </c>
-      <c r="J34" s="1">
+      <c r="J34" s="3">
         <v>100.0</v>
       </c>
-      <c r="K34" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L34" s="1" t="s">
+      <c r="K34" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M34" s="1" t="s">
+      <c r="L34" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N34" s="1" t="s">
+      <c r="M34" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O34" s="1">
+      <c r="N34" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O34" s="3">
         <v>1.76123674997</v>
       </c>
-      <c r="P34" s="1">
+      <c r="P34" s="3">
         <v>968.243447194</v>
       </c>
-      <c r="R34" s="1">
+      <c r="R34" s="3">
         <v>126.0</v>
       </c>
-      <c r="S34" s="2">
+      <c r="S34" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B35" s="2">
+      <c r="A35" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="4">
         <v>44996.42934027778</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E35" s="1">
+      <c r="C35" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E35" s="3">
         <v>6.61</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G35" s="1">
+      <c r="F35" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G35" s="3">
         <v>66.1</v>
       </c>
-      <c r="H35" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I35" s="1">
+      <c r="H35" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I35" s="3">
         <v>2.0</v>
       </c>
-      <c r="J35" s="1">
+      <c r="J35" s="3">
         <v>100.0</v>
       </c>
-      <c r="K35" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L35" s="1" t="s">
+      <c r="K35" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M35" s="1" t="s">
+      <c r="L35" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N35" s="1" t="s">
+      <c r="M35" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O35" s="1">
+      <c r="N35" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O35" s="3">
         <v>1.83263823983</v>
       </c>
-      <c r="P35" s="1">
+      <c r="P35" s="3">
         <v>1011.24211785</v>
       </c>
-      <c r="R35" s="1">
+      <c r="R35" s="3">
         <v>133.0</v>
       </c>
-      <c r="S35" s="2">
+      <c r="S35" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B36" s="2">
+      <c r="A36" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="4">
         <v>44996.42934027778</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E36" s="1">
+      <c r="C36" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E36" s="3">
         <v>6.6</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G36" s="1">
+      <c r="F36" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G36" s="3">
         <v>66.0</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I36" s="1">
+      <c r="H36" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I36" s="3">
         <v>2.0</v>
       </c>
-      <c r="J36" s="1">
+      <c r="J36" s="3">
         <v>100.0</v>
       </c>
-      <c r="K36" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L36" s="1" t="s">
+      <c r="K36" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M36" s="1" t="s">
+      <c r="L36" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N36" s="1" t="s">
+      <c r="M36" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O36" s="1">
+      <c r="N36" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O36" s="3">
         <v>1.78503724659</v>
       </c>
-      <c r="P36" s="1">
+      <c r="P36" s="3">
         <v>967.148849047</v>
       </c>
-      <c r="R36" s="1">
+      <c r="R36" s="3">
         <v>127.0</v>
       </c>
-      <c r="S36" s="2">
+      <c r="S36" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B37" s="2">
+      <c r="A37" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="4">
         <v>44996.42934027778</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E37" s="1">
+      <c r="C37" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E37" s="3">
         <v>6.86</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G37" s="1">
+      <c r="F37" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G37" s="3">
         <v>68.6</v>
       </c>
-      <c r="H37" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I37" s="1">
+      <c r="H37" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I37" s="3">
         <v>2.0</v>
       </c>
-      <c r="J37" s="1">
+      <c r="J37" s="3">
         <v>100.0</v>
       </c>
-      <c r="K37" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L37" s="1" t="s">
+      <c r="K37" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M37" s="1" t="s">
+      <c r="L37" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N37" s="1" t="s">
+      <c r="M37" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O37" s="1">
+      <c r="N37" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O37" s="3">
         <v>1.80883774321</v>
       </c>
-      <c r="P37" s="1">
+      <c r="P37" s="3">
         <v>982.615996767</v>
       </c>
-      <c r="R37" s="1">
+      <c r="R37" s="3">
         <v>134.0</v>
       </c>
-      <c r="S37" s="2">
+      <c r="S37" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B38" s="2">
+      <c r="A38" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38" s="4">
         <v>44996.42934027778</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E38" s="1">
+      <c r="C38" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E38" s="3">
         <v>6.9</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G38" s="1">
+      <c r="F38" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G38" s="3">
         <v>69.0</v>
       </c>
-      <c r="H38" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I38" s="1">
+      <c r="H38" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I38" s="3">
         <v>2.0</v>
       </c>
-      <c r="J38" s="1">
+      <c r="J38" s="3">
         <v>100.0</v>
       </c>
-      <c r="K38" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L38" s="1" t="s">
+      <c r="K38" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M38" s="1" t="s">
+      <c r="L38" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N38" s="1" t="s">
+      <c r="M38" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O38" s="1">
+      <c r="N38" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O38" s="3">
         <v>1.76123674997</v>
       </c>
-      <c r="P38" s="1">
+      <c r="P38" s="3">
         <v>957.939947254</v>
       </c>
-      <c r="R38" s="1">
+      <c r="R38" s="3">
         <v>132.0</v>
       </c>
-      <c r="S38" s="2">
+      <c r="S38" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B39" s="2">
+      <c r="A39" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39" s="4">
         <v>44996.42934027778</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E39" s="1">
+      <c r="C39" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E39" s="3">
         <v>6.9</v>
       </c>
-      <c r="F39" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G39" s="1">
+      <c r="F39" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G39" s="3">
         <v>69.0</v>
       </c>
-      <c r="H39" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I39" s="1">
+      <c r="H39" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I39" s="3">
         <v>2.0</v>
       </c>
-      <c r="J39" s="1">
+      <c r="J39" s="3">
         <v>100.0</v>
       </c>
-      <c r="K39" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L39" s="1" t="s">
+      <c r="K39" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M39" s="1" t="s">
+      <c r="L39" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N39" s="1" t="s">
+      <c r="M39" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O39" s="1">
+      <c r="N39" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O39" s="3">
         <v>1.66603476348</v>
       </c>
-      <c r="P39" s="1">
+      <c r="P39" s="3">
         <v>855.35706446</v>
       </c>
-      <c r="R39" s="1">
+      <c r="R39" s="3">
         <v>118.0</v>
       </c>
-      <c r="S39" s="2">
+      <c r="S39" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B40" s="2">
+      <c r="A40" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40" s="4">
         <v>44996.42934027778</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E40" s="1">
+      <c r="C40" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E40" s="3">
         <v>6.93</v>
       </c>
-      <c r="F40" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G40" s="1">
+      <c r="F40" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G40" s="3">
         <v>69.3</v>
       </c>
-      <c r="H40" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I40" s="1">
+      <c r="H40" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I40" s="3">
         <v>2.0</v>
       </c>
-      <c r="J40" s="1">
+      <c r="J40" s="3">
         <v>100.0</v>
       </c>
-      <c r="K40" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L40" s="1" t="s">
+      <c r="K40" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M40" s="1" t="s">
+      <c r="L40" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N40" s="1" t="s">
+      <c r="M40" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O40" s="1">
+      <c r="N40" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O40" s="3">
         <v>1.47563079051</v>
       </c>
-      <c r="P40" s="1">
+      <c r="P40" s="3">
         <v>814.547590094</v>
       </c>
-      <c r="R40" s="1">
+      <c r="R40" s="3">
         <v>112.0</v>
       </c>
-      <c r="S40" s="2">
+      <c r="S40" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B41" s="2">
+      <c r="A41" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B41" s="4">
         <v>44996.42934027778</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E41" s="1">
+      <c r="C41" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E41" s="3">
         <v>6.84</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G41" s="1">
+      <c r="F41" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G41" s="3">
         <v>68.4</v>
       </c>
-      <c r="H41" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I41" s="1">
+      <c r="H41" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I41" s="3">
         <v>2.0</v>
       </c>
-      <c r="J41" s="1">
+      <c r="J41" s="3">
         <v>100.0</v>
       </c>
-      <c r="K41" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L41" s="1" t="s">
+      <c r="K41" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M41" s="1" t="s">
+      <c r="L41" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N41" s="1" t="s">
+      <c r="M41" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O41" s="1">
+      <c r="N41" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O41" s="3">
         <v>1.49943128713</v>
       </c>
-      <c r="P41" s="1">
+      <c r="P41" s="3">
         <v>790.63300016</v>
       </c>
-      <c r="R41" s="1">
+      <c r="R41" s="3">
         <v>108.0</v>
       </c>
-      <c r="S41" s="2">
+      <c r="S41" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B42" s="2">
+      <c r="A42" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" s="4">
         <v>44996.429444444446</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E42" s="1">
+      <c r="C42" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E42" s="3">
         <v>6.46</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G42" s="1">
+      <c r="F42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G42" s="3">
         <v>64.6</v>
       </c>
-      <c r="H42" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I42" s="1">
+      <c r="H42" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I42" s="3">
         <v>2.0</v>
       </c>
-      <c r="J42" s="1">
+      <c r="J42" s="3">
         <v>100.0</v>
       </c>
-      <c r="K42" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L42" s="1" t="s">
+      <c r="K42" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M42" s="1" t="s">
+      <c r="L42" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N42" s="1" t="s">
+      <c r="M42" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O42" s="1">
+      <c r="N42" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O42" s="3">
         <v>1.76123674997</v>
       </c>
-      <c r="P42" s="1">
+      <c r="P42" s="3">
         <v>968.243447194</v>
       </c>
-      <c r="R42" s="1">
+      <c r="R42" s="3">
         <v>125.0</v>
       </c>
-      <c r="S42" s="2">
+      <c r="S42" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B43" s="2">
+      <c r="A43" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" s="4">
         <v>44996.429444444446</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E43" s="1">
+      <c r="C43" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E43" s="3">
         <v>6.55</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G43" s="1">
+      <c r="F43" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G43" s="3">
         <v>65.5</v>
       </c>
-      <c r="H43" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I43" s="1">
+      <c r="H43" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I43" s="3">
         <v>2.0</v>
       </c>
-      <c r="J43" s="1">
+      <c r="J43" s="3">
         <v>100.0</v>
       </c>
-      <c r="K43" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L43" s="1" t="s">
+      <c r="K43" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M43" s="1" t="s">
+      <c r="L43" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N43" s="1" t="s">
+      <c r="M43" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O43" s="1">
+      <c r="N43" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O43" s="3">
         <v>1.83263823983</v>
       </c>
-      <c r="P43" s="1">
+      <c r="P43" s="3">
         <v>1011.24211785</v>
       </c>
-      <c r="R43" s="1">
+      <c r="R43" s="3">
         <v>132.0</v>
       </c>
-      <c r="S43" s="2">
+      <c r="S43" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B44" s="2">
+      <c r="A44" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B44" s="4">
         <v>44996.429444444446</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E44" s="1">
+      <c r="C44" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E44" s="3">
         <v>6.75</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G44" s="1">
+      <c r="F44" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G44" s="3">
         <v>67.5</v>
       </c>
-      <c r="H44" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I44" s="1">
+      <c r="H44" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I44" s="3">
         <v>2.0</v>
       </c>
-      <c r="J44" s="1">
+      <c r="J44" s="3">
         <v>100.0</v>
       </c>
-      <c r="K44" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L44" s="1" t="s">
+      <c r="K44" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M44" s="1" t="s">
+      <c r="L44" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N44" s="1" t="s">
+      <c r="M44" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O44" s="1">
+      <c r="N44" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O44" s="3">
         <v>1.78503724659</v>
       </c>
-      <c r="P44" s="1">
+      <c r="P44" s="3">
         <v>967.148849047</v>
       </c>
-      <c r="R44" s="1">
+      <c r="R44" s="3">
         <v>130.0</v>
       </c>
-      <c r="S44" s="2">
+      <c r="S44" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B45" s="2">
+      <c r="A45" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B45" s="4">
         <v>44996.429444444446</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E45" s="1">
+      <c r="C45" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E45" s="3">
         <v>6.98</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G45" s="1">
+      <c r="F45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G45" s="3">
         <v>69.8</v>
       </c>
-      <c r="H45" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I45" s="1">
+      <c r="H45" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I45" s="3">
         <v>2.0</v>
       </c>
-      <c r="J45" s="1">
+      <c r="J45" s="3">
         <v>100.0</v>
       </c>
-      <c r="K45" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L45" s="1" t="s">
+      <c r="K45" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M45" s="1" t="s">
+      <c r="L45" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N45" s="1" t="s">
+      <c r="M45" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O45" s="1">
+      <c r="N45" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O45" s="3">
         <v>1.80883774321</v>
       </c>
-      <c r="P45" s="1">
+      <c r="P45" s="3">
         <v>982.615996767</v>
       </c>
-      <c r="R45" s="1">
+      <c r="R45" s="3">
         <v>137.0</v>
       </c>
-      <c r="S45" s="2">
+      <c r="S45" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B46" s="2">
+      <c r="A46" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46" s="4">
         <v>44996.429444444446</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E46" s="1">
+      <c r="C46" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E46" s="3">
         <v>6.81</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G46" s="1">
+      <c r="F46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G46" s="3">
         <v>68.1</v>
       </c>
-      <c r="H46" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I46" s="1">
+      <c r="H46" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I46" s="3">
         <v>2.0</v>
       </c>
-      <c r="J46" s="1">
+      <c r="J46" s="3">
         <v>100.0</v>
       </c>
-      <c r="K46" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L46" s="1" t="s">
+      <c r="K46" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M46" s="1" t="s">
+      <c r="L46" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N46" s="1" t="s">
+      <c r="M46" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O46" s="1">
+      <c r="N46" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O46" s="3">
         <v>1.76123674997</v>
       </c>
-      <c r="P46" s="1">
+      <c r="P46" s="3">
         <v>957.939947254</v>
       </c>
-      <c r="R46" s="1">
+      <c r="R46" s="3">
         <v>130.0</v>
       </c>
-      <c r="S46" s="2">
+      <c r="S46" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B47" s="2">
+      <c r="A47" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" s="4">
         <v>44996.429444444446</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E47" s="1">
+      <c r="C47" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E47" s="3">
         <v>6.74</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G47" s="1">
+      <c r="F47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G47" s="3">
         <v>67.4</v>
       </c>
-      <c r="H47" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I47" s="1">
+      <c r="H47" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I47" s="3">
         <v>2.0</v>
       </c>
-      <c r="J47" s="1">
+      <c r="J47" s="3">
         <v>100.0</v>
       </c>
-      <c r="K47" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L47" s="1" t="s">
+      <c r="K47" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M47" s="1" t="s">
+      <c r="L47" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N47" s="1" t="s">
+      <c r="M47" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O47" s="1">
+      <c r="N47" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O47" s="3">
         <v>1.66603476348</v>
       </c>
-      <c r="P47" s="1">
+      <c r="P47" s="3">
         <v>855.35706446</v>
       </c>
-      <c r="R47" s="1">
+      <c r="R47" s="3">
         <v>115.0</v>
       </c>
-      <c r="S47" s="2">
+      <c r="S47" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B48" s="2">
+      <c r="A48" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B48" s="4">
         <v>44996.429444444446</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E48" s="1">
+      <c r="C48" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E48" s="3">
         <v>6.92</v>
       </c>
-      <c r="F48" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G48" s="1">
+      <c r="F48" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G48" s="3">
         <v>69.2</v>
       </c>
-      <c r="H48" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I48" s="1">
+      <c r="H48" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I48" s="3">
         <v>2.0</v>
       </c>
-      <c r="J48" s="1">
+      <c r="J48" s="3">
         <v>100.0</v>
       </c>
-      <c r="K48" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L48" s="1" t="s">
+      <c r="K48" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M48" s="1" t="s">
+      <c r="L48" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N48" s="1" t="s">
+      <c r="M48" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O48" s="1">
+      <c r="N48" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O48" s="3">
         <v>1.47563079051</v>
       </c>
-      <c r="P48" s="1">
+      <c r="P48" s="3">
         <v>814.547590094</v>
       </c>
-      <c r="R48" s="1">
+      <c r="R48" s="3">
         <v>112.0</v>
       </c>
-      <c r="S48" s="2">
+      <c r="S48" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B49" s="2">
+      <c r="A49" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B49" s="4">
         <v>44996.429444444446</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E49" s="1">
+      <c r="C49" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E49" s="3">
         <v>6.76</v>
       </c>
-      <c r="F49" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G49" s="1">
+      <c r="F49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G49" s="3">
         <v>67.6</v>
       </c>
-      <c r="H49" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I49" s="1">
+      <c r="H49" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I49" s="3">
         <v>2.0</v>
       </c>
-      <c r="J49" s="1">
+      <c r="J49" s="3">
         <v>100.0</v>
       </c>
-      <c r="K49" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L49" s="1" t="s">
+      <c r="K49" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M49" s="1" t="s">
+      <c r="L49" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N49" s="1" t="s">
+      <c r="M49" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O49" s="1">
+      <c r="N49" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O49" s="3">
         <v>1.49943128713</v>
       </c>
-      <c r="P49" s="1">
+      <c r="P49" s="3">
         <v>790.63300016</v>
       </c>
-      <c r="R49" s="1">
+      <c r="R49" s="3">
         <v>107.0</v>
       </c>
-      <c r="S49" s="2">
+      <c r="S49" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
@@ -4263,414 +4277,411 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
-  <cols>
-    <col customWidth="1" min="1" max="6" width="12.63"/>
-  </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="W1" s="3" t="s">
         <v>22</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="A2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="4">
         <v>44996.42888888889</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="1">
+      <c r="D2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="3">
         <v>8.09</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G2" s="1">
+      <c r="F2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="3">
         <v>80.9</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="1">
+      <c r="H2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="3">
         <v>2.0</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="3">
         <v>100.0</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="K2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="L2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="M2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O2" s="1">
+      <c r="N2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="3">
         <v>1.76123674997</v>
       </c>
-      <c r="P2" s="1">
+      <c r="P2" s="3">
         <v>968.243447194</v>
       </c>
-      <c r="R2" s="1">
+      <c r="R2" s="3">
         <v>156.0</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="A3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="4">
         <v>44996.42888888889</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="C3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="3">
+        <v>8.15</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="3">
+        <v>81.5</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="J3" s="3">
+        <v>100.0</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="1">
-        <v>8.15</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="1">
-        <v>81.5</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="J3" s="1">
-        <v>100.0</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O3" s="1">
+      <c r="O3" s="3">
         <v>1.83263823983</v>
       </c>
-      <c r="P3" s="1">
+      <c r="P3" s="3">
         <v>1011.24211785</v>
       </c>
-      <c r="R3" s="1">
+      <c r="R3" s="3">
         <v>164.0</v>
       </c>
-      <c r="S3" s="2">
+      <c r="S3" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="A4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="4">
         <v>44996.42888888889</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="1">
+      <c r="C4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="3">
         <v>8.1</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="1">
+      <c r="F4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="3">
         <v>81.0</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="1">
+      <c r="H4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="3">
         <v>2.0</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="3">
         <v>100.0</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" s="1" t="s">
+      <c r="K4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="L4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="M4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O4" s="1">
+      <c r="N4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" s="3">
         <v>1.78503724659</v>
       </c>
-      <c r="P4" s="1">
+      <c r="P4" s="3">
         <v>967.148849047</v>
       </c>
-      <c r="R4" s="1">
+      <c r="R4" s="3">
         <v>156.0</v>
       </c>
-      <c r="S4" s="2">
+      <c r="S4" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="A5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="4">
         <v>44996.42888888889</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="1">
+      <c r="C5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="3">
         <v>8.27</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="1">
+      <c r="F5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="3">
         <v>82.7</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I5" s="1">
+      <c r="H5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="3">
         <v>2.0</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="3">
         <v>100.0</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L5" s="1" t="s">
+      <c r="K5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="L5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="M5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O5" s="1">
+      <c r="N5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5" s="3">
         <v>1.80883774321</v>
       </c>
-      <c r="P5" s="1">
+      <c r="P5" s="3">
         <v>982.615996767</v>
       </c>
-      <c r="R5" s="1">
+      <c r="R5" s="3">
         <v>162.0</v>
       </c>
-      <c r="S5" s="2">
+      <c r="S5" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="2">
+      <c r="A6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="4">
         <v>44996.42888888889</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="1">
+      <c r="C6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="3">
         <v>7.85</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="1">
+      <c r="F6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="3">
         <v>78.5</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="1">
+      <c r="H6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="3">
         <v>2.0</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="3">
         <v>100.0</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L6" s="1" t="s">
+      <c r="K6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="L6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="M6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O6" s="1">
+      <c r="N6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O6" s="3">
         <v>1.76123674997</v>
       </c>
-      <c r="P6" s="1">
+      <c r="P6" s="3">
         <v>957.939947254</v>
       </c>
-      <c r="R6" s="1">
+      <c r="R6" s="3">
         <v>150.0</v>
       </c>
-      <c r="S6" s="2">
+      <c r="S6" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="2">
+      <c r="A7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="4">
         <v>44996.42888888889</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="1">
+      <c r="C7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="3">
         <v>7.75</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="1">
+      <c r="F7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="3">
         <v>77.5</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I7" s="1">
+      <c r="H7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="3">
         <v>2.0</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="3">
         <v>100.0</v>
       </c>
-      <c r="K7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L7" s="1" t="s">
+      <c r="K7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="L7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="M7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O7" s="1">
+      <c r="N7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O7" s="3">
         <v>1.66603476348</v>
       </c>
-      <c r="P7" s="1">
+      <c r="P7" s="3">
         <v>855.35706446</v>
       </c>
-      <c r="R7" s="1">
+      <c r="R7" s="3">
         <v>132.0</v>
       </c>
-      <c r="S7" s="2">
+      <c r="S7" s="4">
         <v>44968.44994212963</v>
       </c>
     </row>

</xml_diff>